<commit_message>
tfp job queue status change
</commit_message>
<xml_diff>
--- a/GFM-Daily-Job-Queue-Entries-Monitor-Report-Jan-2024.xlsx
+++ b/GFM-Daily-Job-Queue-Entries-Monitor-Report-Jan-2024.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah.nadim\Desktop\Nadim_Work\UiPath\RPAITProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88929D06-F783-4464-9F76-923BBA67CFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9E27FB-C520-4B2C-8353-4C10E9084415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Job Queue Entries" sheetId="1" r:id="rId1"/>
+    <sheet name="29-01-2024" sheetId="3" r:id="rId1"/>
+    <sheet name="26-01-2024" sheetId="2" r:id="rId2"/>
+    <sheet name="01-01-2024" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="59">
   <si>
     <t>Status</t>
   </si>
@@ -128,7 +130,28 @@
     <t>C ACIE - #1 Adjust Cost - Item Entries</t>
   </si>
   <si>
-    <t>Error</t>
+    <t>LS Scheduler Service</t>
+  </si>
+  <si>
+    <t>C B2B - Inbound_SI</t>
+  </si>
+  <si>
+    <t>LSSCHEDULE</t>
+  </si>
+  <si>
+    <t>Post Inventory Cost to G/L</t>
+  </si>
+  <si>
+    <t>C ACIE - #2 Post Inventory Cost to G/L</t>
+  </si>
+  <si>
+    <t>FP\RPA</t>
+  </si>
+  <si>
+    <t>TFP - NAS &amp; Batch Svc Monitor</t>
+  </si>
+  <si>
+    <t>C TFP - NAS &amp; Batch Svc Monitor</t>
   </si>
   <si>
     <t>TFP - Job Queue Monitor</t>
@@ -137,28 +160,58 @@
     <t>C TFP - Job Queue Monitor</t>
   </si>
   <si>
-    <t>LS Scheduler Service</t>
-  </si>
-  <si>
-    <t>C B2B - Inbound_SI</t>
-  </si>
-  <si>
-    <t>LSSCHEDULE</t>
-  </si>
-  <si>
-    <t>Post Inventory Cost to G/L</t>
-  </si>
-  <si>
-    <t>C ACIE - #2 Post Inventory Cost to G/L</t>
-  </si>
-  <si>
-    <t>FP\RPA</t>
-  </si>
-  <si>
-    <t>TFP - NAS &amp; Batch Svc Monitor</t>
-  </si>
-  <si>
-    <t>C TFP - NAS &amp; Batch Svc Monitor</t>
+    <t>27/01/24 08:00:00</t>
+  </si>
+  <si>
+    <t>27/01/24 06:30:00</t>
+  </si>
+  <si>
+    <t>27/01/24 06:00:00</t>
+  </si>
+  <si>
+    <t>27/01/24 03:00:00</t>
+  </si>
+  <si>
+    <t>26/01/24 21:40:00</t>
+  </si>
+  <si>
+    <t>26/01/24 23:00:00</t>
+  </si>
+  <si>
+    <t>26/01/24 10:15:31</t>
+  </si>
+  <si>
+    <t>26/01/24 11:05:41</t>
+  </si>
+  <si>
+    <t>26/01/24 10:16:49</t>
+  </si>
+  <si>
+    <t>30/01/24 08:00:00</t>
+  </si>
+  <si>
+    <t>30/01/24 06:30:00</t>
+  </si>
+  <si>
+    <t>30/01/24 06:00:00</t>
+  </si>
+  <si>
+    <t>30/01/24 03:00:00</t>
+  </si>
+  <si>
+    <t>29/01/24 21:40:00</t>
+  </si>
+  <si>
+    <t>29/01/24 10:41:29</t>
+  </si>
+  <si>
+    <t>29/01/24 23:00:00</t>
+  </si>
+  <si>
+    <t>29/01/24 11:03:29</t>
+  </si>
+  <si>
+    <t>29/01/24 10:34:32</t>
   </si>
 </sst>
 </file>
@@ -254,9 +307,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +347,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -400,7 +453,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,19 +595,831 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BAE0ECD-15F5-407C-BA15-FA5CA6672F73}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>50099</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>50007</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>50011</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>50000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>50010</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>50015</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>795</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>99001469</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1002</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>50097</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>50096</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BD95F7-791D-427F-A67C-8EF4896C0166}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>50099</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>50007</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>50011</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>50000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>50010</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>50015</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>795</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>99001469</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1002</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>50097</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>50096</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,7 +1500,7 @@
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4">
-        <v>45315.333333333299</v>
+        <v>45316.333333333299</v>
       </c>
       <c r="J2" s="3" t="b">
         <f>TRUE()</f>
@@ -673,7 +1538,7 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4">
-        <v>45315.270833333299</v>
+        <v>45316.270833333299</v>
       </c>
       <c r="J3" s="3" t="b">
         <f>TRUE()</f>
@@ -711,7 +1576,7 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4">
-        <v>45315.25</v>
+        <v>45316.25</v>
       </c>
       <c r="J4" s="3" t="b">
         <f>TRUE()</f>
@@ -749,7 +1614,7 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4">
-        <v>45315.25</v>
+        <v>45316.25</v>
       </c>
       <c r="J5" s="3" t="b">
         <f>TRUE()</f>
@@ -787,7 +1652,7 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4">
-        <v>45315.25</v>
+        <v>45316.25</v>
       </c>
       <c r="J6" s="3" t="b">
         <f>TRUE()</f>
@@ -825,7 +1690,7 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4">
-        <v>45315.125</v>
+        <v>45316.125</v>
       </c>
       <c r="J7" s="3" t="b">
         <f>TRUE()</f>
@@ -863,7 +1728,7 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4">
-        <v>45314.902777777803</v>
+        <v>45315.902777777803</v>
       </c>
       <c r="J8" s="3" t="b">
         <f>TRUE()</f>
@@ -879,40 +1744,40 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>99001469</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3">
-        <v>50097</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4">
-        <v>45310.711223414299</v>
+        <v>45315.650912580997</v>
       </c>
       <c r="J9" s="3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K9" s="3" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="L9" s="3">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -923,10 +1788,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3">
-        <v>99001469</v>
+        <v>1002</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>34</v>
@@ -935,11 +1800,11 @@
         <v>35</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4">
-        <v>45314.804845023202</v>
+        <v>45315.958333333299</v>
       </c>
       <c r="J10" s="3" t="b">
         <f>TRUE()</f>
@@ -950,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -958,13 +1823,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <v>1002</v>
+        <v>50096</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>37</v>
@@ -977,7 +1842,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4">
-        <v>45314.958333333299</v>
+        <v>45315.643746330999</v>
       </c>
       <c r="J11" s="3" t="b">
         <f>TRUE()</f>
@@ -988,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -996,26 +1861,26 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="3">
-        <v>50096</v>
+        <v>50097</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4">
-        <v>45314.797358830998</v>
+        <v>45315.673088738396</v>
       </c>
       <c r="J12" s="3" t="b">
         <f>TRUE()</f>
@@ -1026,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="3">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>